<commit_message>
Settati i test 6,9,147,150 come non applicabili, in quanto sono richiesti degli elementi opzionali non implementati in Human Eseguiti nuovamente i test sul JWT, 29,32,37,40
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111BIMIND00000/BiMind/Human/10.6/report-checklist.xlsx
+++ b/GATEWAY/A1#111BIMIND00000/BiMind/Human/10.6/report-checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\ProgettiGit\it-fse-accreditamento\GATEWAY\A1#111BIMIND00000\BiMind\Human\10.6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53BA7572-F0A7-48A0-9027-E6F3A6432B5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D03C9E23-CBDA-4690-A097-4871A858A690}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15855" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="242">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -819,43 +819,13 @@
     <t>Non viene gestito il dato strutturato relativa alla data di insorgenza del problema indicato nell'anamnesi patologica prossima o remota</t>
   </si>
   <si>
-    <t>8547885f1428158c</t>
-  </si>
-  <si>
-    <t>2023-03-24T10:45:43Z</t>
-  </si>
-  <si>
     <t>La generazione del JWT viene corretta e il documento validato a posteriori</t>
   </si>
   <si>
-    <t>89a1a10e81fca573</t>
-  </si>
-  <si>
-    <t>2023-03-24T10:56:08Z</t>
-  </si>
-  <si>
     <t>Errore connessione al servizio di validazione del documento. Verrà ritentata la validazione a breve. Proseguire con la firma</t>
   </si>
   <si>
     <t xml:space="preserve"> Visualizzazione errore di connessione al servizio all'operatore. La validazione verrà ritentata in background a posteriori</t>
-  </si>
-  <si>
-    <t>f773766e72fbd443</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.10.4.4.cb075905a8bb4b972ef1bc42d64d35cae189f6e38c37fcf438950d1782f28bd9.bfcbf6020e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-03-24T11:22:37Z</t>
-  </si>
-  <si>
-    <t>166ab5d17ffaae6e</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.10.4.4.8b4826fc860c5c74e62ab4402d484841b0a42d9a3b46888e4a2067f77607fabf.3be272a8bb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-03-24T11:30:07Z</t>
   </si>
   <si>
     <t>03093a48ffc66c8e</t>
@@ -994,36 +964,6 @@
     <t>2023-03-24T01:29:37Z</t>
   </si>
   <si>
-    <t>bb09f9497d1671c1</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.110.4.4.e855fe5e6ea5ff1364867dbdb0d6ed8358ea22af8eaa1f63dbde46ce3faaa3fb.5ad729947c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-03-25T12:23:25Z</t>
-  </si>
-  <si>
-    <t>42585c52b28d53b6</t>
-  </si>
-  <si>
-    <t>2023-03-25T12:32:06Z</t>
-  </si>
-  <si>
-    <t>9c38639423e64e84</t>
-  </si>
-  <si>
-    <t>2023-03-25T12:35:18Z</t>
-  </si>
-  <si>
-    <t>f3e2cdf75686c4de</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.110.4.4.1861ec98c8dfdab112ff521e7cc18da5dfc65360e2b6f21a2f0af25ecd0c15f6.6db9cd8cd4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-03-25T12:44:13Z</t>
-  </si>
-  <si>
     <t>bbbe12fd497169c8</t>
   </si>
   <si>
@@ -1091,6 +1031,30 @@
   </si>
   <si>
     <t>L'operatore deve valorizzare il decorso ospedaliero e ricreare la stampa</t>
+  </si>
+  <si>
+    <t>d03122037f8fcf0b</t>
+  </si>
+  <si>
+    <t>2023-04-20T12:12:21Z</t>
+  </si>
+  <si>
+    <t>e06f457d76c74fef</t>
+  </si>
+  <si>
+    <t>2023-04-20T12:14:55Z</t>
+  </si>
+  <si>
+    <t>0a939c5b5387ac96</t>
+  </si>
+  <si>
+    <t>2023-04-20T12:17:24Z</t>
+  </si>
+  <si>
+    <t>9397f520b13e559f</t>
+  </si>
+  <si>
+    <t>2023-04-20T12:19:20Z</t>
   </si>
 </sst>
 </file>
@@ -1871,7 +1835,7 @@
     </row>
     <row r="4" spans="1:1" ht="14.25" customHeight="1">
       <c r="A4" s="37" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="14.25" customHeight="1">
@@ -4010,10 +3974,10 @@
   <dimension ref="A1:T672"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="P27" sqref="P27"/>
+      <selection pane="bottomRight" activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -4283,30 +4247,22 @@
       <c r="E10" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="F10" s="23">
-        <v>45010</v>
-      </c>
-      <c r="G10" s="24" t="s">
-        <v>223</v>
-      </c>
-      <c r="H10" s="24" t="s">
-        <v>221</v>
-      </c>
-      <c r="I10" s="24" t="s">
-        <v>222</v>
-      </c>
+      <c r="F10" s="23"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
       <c r="J10" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="K10" s="25"/>
+        <v>146</v>
+      </c>
+      <c r="K10" s="32" t="s">
+        <v>161</v>
+      </c>
       <c r="L10" s="25"/>
       <c r="M10" s="25"/>
       <c r="N10" s="25"/>
       <c r="O10" s="25"/>
       <c r="P10" s="25"/>
-      <c r="Q10" s="25" t="s">
-        <v>144</v>
-      </c>
+      <c r="Q10" s="25"/>
       <c r="R10" s="26"/>
       <c r="S10" s="27"/>
       <c r="T10" s="28" t="s">
@@ -4405,30 +4361,22 @@
       <c r="E13" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="F13" s="23">
-        <v>45010</v>
-      </c>
-      <c r="G13" s="24" t="s">
-        <v>230</v>
-      </c>
-      <c r="H13" s="24" t="s">
-        <v>228</v>
-      </c>
-      <c r="I13" s="24" t="s">
-        <v>229</v>
-      </c>
+      <c r="F13" s="23"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
       <c r="J13" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="K13" s="25"/>
+        <v>146</v>
+      </c>
+      <c r="K13" s="32" t="s">
+        <v>161</v>
+      </c>
       <c r="L13" s="25"/>
       <c r="M13" s="25"/>
       <c r="N13" s="25"/>
       <c r="O13" s="25"/>
       <c r="P13" s="25"/>
-      <c r="Q13" s="25" t="s">
-        <v>144</v>
-      </c>
+      <c r="Q13" s="25"/>
       <c r="R13" s="26"/>
       <c r="S13" s="27"/>
       <c r="T13" s="28" t="s">
@@ -4452,13 +4400,13 @@
         <v>57</v>
       </c>
       <c r="F14" s="23">
-        <v>45010</v>
+        <v>45036</v>
       </c>
       <c r="G14" s="24" t="s">
-        <v>225</v>
+        <v>239</v>
       </c>
       <c r="H14" s="24" t="s">
-        <v>224</v>
+        <v>238</v>
       </c>
       <c r="I14" s="24"/>
       <c r="J14" s="25" t="s">
@@ -4466,7 +4414,7 @@
       </c>
       <c r="K14" s="25"/>
       <c r="L14" s="25" t="s">
-        <v>146</v>
+        <v>64</v>
       </c>
       <c r="M14" s="25" t="s">
         <v>146</v>
@@ -4476,7 +4424,7 @@
         <v>64</v>
       </c>
       <c r="P14" s="25" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="Q14" s="25" t="s">
         <v>144</v>
@@ -4504,13 +4452,13 @@
         <v>57</v>
       </c>
       <c r="F15" s="23">
-        <v>45009</v>
+        <v>45036</v>
       </c>
       <c r="G15" s="24" t="s">
-        <v>167</v>
+        <v>235</v>
       </c>
       <c r="H15" s="24" t="s">
-        <v>166</v>
+        <v>234</v>
       </c>
       <c r="I15" s="24"/>
       <c r="J15" s="25" t="s">
@@ -4518,7 +4466,7 @@
       </c>
       <c r="K15" s="25"/>
       <c r="L15" s="25" t="s">
-        <v>146</v>
+        <v>64</v>
       </c>
       <c r="M15" s="25" t="s">
         <v>146</v>
@@ -4528,7 +4476,7 @@
         <v>64</v>
       </c>
       <c r="P15" s="25" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="Q15" s="25" t="s">
         <v>144</v>
@@ -4556,13 +4504,13 @@
         <v>60</v>
       </c>
       <c r="F16" s="23">
-        <v>45010</v>
+        <v>45036</v>
       </c>
       <c r="G16" s="24" t="s">
-        <v>227</v>
+        <v>241</v>
       </c>
       <c r="H16" s="24" t="s">
-        <v>226</v>
+        <v>240</v>
       </c>
       <c r="I16" s="24"/>
       <c r="J16" s="25" t="s">
@@ -4570,7 +4518,7 @@
       </c>
       <c r="K16" s="25"/>
       <c r="L16" s="25" t="s">
-        <v>146</v>
+        <v>64</v>
       </c>
       <c r="M16" s="25" t="s">
         <v>146</v>
@@ -4580,7 +4528,7 @@
         <v>64</v>
       </c>
       <c r="P16" s="25" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="Q16" s="25" t="s">
         <v>144</v>
@@ -4608,13 +4556,13 @@
         <v>62</v>
       </c>
       <c r="F17" s="23">
-        <v>45009</v>
+        <v>45036</v>
       </c>
       <c r="G17" s="24" t="s">
-        <v>170</v>
+        <v>237</v>
       </c>
       <c r="H17" s="24" t="s">
-        <v>169</v>
+        <v>236</v>
       </c>
       <c r="I17" s="24"/>
       <c r="J17" s="25" t="s">
@@ -4622,7 +4570,7 @@
       </c>
       <c r="K17" s="25"/>
       <c r="L17" s="25" t="s">
-        <v>146</v>
+        <v>64</v>
       </c>
       <c r="M17" s="25" t="s">
         <v>146</v>
@@ -4632,7 +4580,7 @@
         <v>64</v>
       </c>
       <c r="P17" s="25" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="Q17" s="25" t="s">
         <v>144</v>
@@ -4674,13 +4622,13 @@
         <v>64</v>
       </c>
       <c r="N18" s="25" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="O18" s="25" t="s">
         <v>64</v>
       </c>
       <c r="P18" s="25" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="Q18" s="25" t="s">
         <v>144</v>
@@ -4724,13 +4672,13 @@
         <v>64</v>
       </c>
       <c r="N19" s="25" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="O19" s="25" t="s">
         <v>64</v>
       </c>
       <c r="P19" s="25" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="Q19" s="25" t="s">
         <v>144</v>
@@ -4763,13 +4711,13 @@
         <v>45010</v>
       </c>
       <c r="G20" s="24" t="s">
-        <v>233</v>
+        <v>213</v>
       </c>
       <c r="H20" s="24" t="s">
-        <v>231</v>
+        <v>211</v>
       </c>
       <c r="I20" s="24" t="s">
-        <v>232</v>
+        <v>212</v>
       </c>
       <c r="J20" s="25" t="s">
         <v>64</v>
@@ -4782,13 +4730,13 @@
         <v>64</v>
       </c>
       <c r="N20" s="25" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="O20" s="25" t="s">
         <v>146</v>
       </c>
       <c r="P20" s="25" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="Q20" s="25" t="s">
         <v>144</v>
@@ -4819,13 +4767,13 @@
         <v>45010</v>
       </c>
       <c r="G21" s="24" t="s">
-        <v>236</v>
+        <v>216</v>
       </c>
       <c r="H21" s="24" t="s">
-        <v>234</v>
+        <v>214</v>
       </c>
       <c r="I21" s="24" t="s">
-        <v>235</v>
+        <v>215</v>
       </c>
       <c r="J21" s="25" t="s">
         <v>64</v>
@@ -4838,13 +4786,13 @@
         <v>64</v>
       </c>
       <c r="N21" s="25" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="O21" s="25" t="s">
         <v>146</v>
       </c>
       <c r="P21" s="25" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="Q21" s="25" t="s">
         <v>144</v>
@@ -4875,13 +4823,13 @@
         <v>45010</v>
       </c>
       <c r="G22" s="24" t="s">
-        <v>239</v>
+        <v>219</v>
       </c>
       <c r="H22" s="24" t="s">
-        <v>237</v>
+        <v>217</v>
       </c>
       <c r="I22" s="24" t="s">
-        <v>238</v>
+        <v>218</v>
       </c>
       <c r="J22" s="25" t="s">
         <v>64</v>
@@ -4894,13 +4842,13 @@
         <v>64</v>
       </c>
       <c r="N22" s="25" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="O22" s="25" t="s">
         <v>146</v>
       </c>
       <c r="P22" s="25" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="Q22" s="25" t="s">
         <v>144</v>
@@ -4969,13 +4917,13 @@
         <v>45010</v>
       </c>
       <c r="G24" s="24" t="s">
-        <v>242</v>
+        <v>222</v>
       </c>
       <c r="H24" s="24" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="I24" s="24" t="s">
-        <v>241</v>
+        <v>221</v>
       </c>
       <c r="J24" s="25" t="s">
         <v>64</v>
@@ -4988,13 +4936,13 @@
         <v>64</v>
       </c>
       <c r="N24" s="25" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="O24" s="25" t="s">
         <v>146</v>
       </c>
       <c r="P24" s="25" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="Q24" s="25" t="s">
         <v>144</v>
@@ -5025,13 +4973,13 @@
         <v>45010</v>
       </c>
       <c r="G25" s="24" t="s">
-        <v>244</v>
+        <v>224</v>
       </c>
       <c r="H25" s="24" t="s">
-        <v>243</v>
+        <v>223</v>
       </c>
       <c r="I25" s="24" t="s">
-        <v>245</v>
+        <v>225</v>
       </c>
       <c r="J25" s="25" t="s">
         <v>64</v>
@@ -5044,13 +4992,13 @@
         <v>64</v>
       </c>
       <c r="N25" s="33" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="O25" s="25" t="s">
         <v>146</v>
       </c>
       <c r="P25" s="25" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="Q25" s="25" t="s">
         <v>144</v>
@@ -5081,13 +5029,13 @@
         <v>45010</v>
       </c>
       <c r="G26" s="24" t="s">
-        <v>247</v>
+        <v>227</v>
       </c>
       <c r="H26" s="24" t="s">
-        <v>246</v>
+        <v>226</v>
       </c>
       <c r="I26" s="24" t="s">
-        <v>248</v>
+        <v>228</v>
       </c>
       <c r="J26" s="25" t="s">
         <v>64</v>
@@ -5100,13 +5048,13 @@
         <v>64</v>
       </c>
       <c r="N26" s="33" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="O26" s="25" t="s">
         <v>146</v>
       </c>
       <c r="P26" s="33" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="Q26" s="25" t="s">
         <v>144</v>
@@ -5137,13 +5085,13 @@
         <v>45010</v>
       </c>
       <c r="G27" s="24" t="s">
-        <v>250</v>
+        <v>230</v>
       </c>
       <c r="H27" s="24" t="s">
-        <v>249</v>
+        <v>229</v>
       </c>
       <c r="I27" s="24" t="s">
-        <v>251</v>
+        <v>231</v>
       </c>
       <c r="J27" s="25" t="s">
         <v>64</v>
@@ -5156,13 +5104,13 @@
         <v>64</v>
       </c>
       <c r="N27" s="33" t="s">
-        <v>252</v>
+        <v>232</v>
       </c>
       <c r="O27" s="25" t="s">
         <v>146</v>
       </c>
       <c r="P27" s="33" t="s">
-        <v>253</v>
+        <v>233</v>
       </c>
       <c r="Q27" s="25" t="s">
         <v>144</v>
@@ -5341,30 +5289,22 @@
       <c r="E32" s="22" t="s">
         <v>92</v>
       </c>
-      <c r="F32" s="23">
-        <v>45009</v>
-      </c>
-      <c r="G32" s="24" t="s">
-        <v>175</v>
-      </c>
-      <c r="H32" s="24" t="s">
-        <v>173</v>
-      </c>
-      <c r="I32" s="24" t="s">
-        <v>174</v>
-      </c>
+      <c r="F32" s="23"/>
+      <c r="G32" s="24"/>
+      <c r="H32" s="24"/>
+      <c r="I32" s="24"/>
       <c r="J32" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="K32" s="25"/>
+        <v>146</v>
+      </c>
+      <c r="K32" s="25" t="s">
+        <v>161</v>
+      </c>
       <c r="L32" s="25"/>
       <c r="M32" s="25"/>
       <c r="N32" s="25"/>
       <c r="O32" s="25"/>
       <c r="P32" s="25"/>
-      <c r="Q32" s="25" t="s">
-        <v>144</v>
-      </c>
+      <c r="Q32" s="25"/>
       <c r="R32" s="26"/>
       <c r="S32" s="27"/>
       <c r="T32" s="28" t="s">
@@ -5463,30 +5403,22 @@
       <c r="E35" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="F35" s="23">
-        <v>45009</v>
-      </c>
-      <c r="G35" s="34" t="s">
-        <v>178</v>
-      </c>
-      <c r="H35" s="24" t="s">
-        <v>176</v>
-      </c>
-      <c r="I35" s="24" t="s">
-        <v>177</v>
-      </c>
+      <c r="F35" s="23"/>
+      <c r="G35" s="34"/>
+      <c r="H35" s="24"/>
+      <c r="I35" s="24"/>
       <c r="J35" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="K35" s="25"/>
+        <v>146</v>
+      </c>
+      <c r="K35" s="25" t="s">
+        <v>161</v>
+      </c>
       <c r="L35" s="25"/>
       <c r="M35" s="25"/>
       <c r="N35" s="25"/>
       <c r="O35" s="25"/>
       <c r="P35" s="25"/>
-      <c r="Q35" s="25" t="s">
-        <v>144</v>
-      </c>
+      <c r="Q35" s="25"/>
       <c r="R35" s="26"/>
       <c r="S35" s="27"/>
       <c r="T35" s="28" t="s">
@@ -5513,13 +5445,13 @@
         <v>45009</v>
       </c>
       <c r="G36" s="24" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="H36" s="24" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="I36" s="24" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="J36" s="25" t="s">
         <v>64</v>
@@ -5532,13 +5464,13 @@
         <v>64</v>
       </c>
       <c r="N36" s="25" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="O36" s="25" t="s">
         <v>146</v>
       </c>
       <c r="P36" s="25" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="Q36" s="25" t="s">
         <v>144</v>
@@ -5569,13 +5501,13 @@
         <v>45009</v>
       </c>
       <c r="G37" s="24" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="H37" s="24" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="I37" s="24" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="J37" s="25" t="s">
         <v>64</v>
@@ -5588,13 +5520,13 @@
         <v>64</v>
       </c>
       <c r="N37" s="25" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="O37" s="25" t="s">
         <v>146</v>
       </c>
       <c r="P37" s="25" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="Q37" s="25" t="s">
         <v>144</v>
@@ -5625,13 +5557,13 @@
         <v>45009</v>
       </c>
       <c r="G38" s="24" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="H38" s="24" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="I38" s="24" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="J38" s="25" t="s">
         <v>64</v>
@@ -5644,13 +5576,13 @@
         <v>64</v>
       </c>
       <c r="N38" s="25" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="O38" s="25" t="s">
         <v>146</v>
       </c>
       <c r="P38" s="25" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="Q38" s="25" t="s">
         <v>144</v>
@@ -5719,13 +5651,13 @@
         <v>45009</v>
       </c>
       <c r="G40" s="24" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="H40" s="24" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="I40" s="24" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="J40" s="25" t="s">
         <v>64</v>
@@ -5738,13 +5670,13 @@
         <v>64</v>
       </c>
       <c r="N40" s="25" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="O40" s="25" t="s">
         <v>146</v>
       </c>
       <c r="P40" s="25" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="Q40" s="25" t="s">
         <v>144</v>
@@ -5775,13 +5707,13 @@
         <v>45009</v>
       </c>
       <c r="G41" s="24" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="H41" s="24" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="I41" s="24" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="J41" s="25" t="s">
         <v>64</v>
@@ -5794,13 +5726,13 @@
         <v>64</v>
       </c>
       <c r="N41" s="33" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="O41" s="25" t="s">
         <v>146</v>
       </c>
       <c r="P41" s="25" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="Q41" s="25" t="s">
         <v>144</v>
@@ -5945,13 +5877,13 @@
         <v>45009</v>
       </c>
       <c r="G45" s="24" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="H45" s="24" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="I45" s="24" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="J45" s="25" t="s">
         <v>64</v>
@@ -5964,13 +5896,13 @@
         <v>64</v>
       </c>
       <c r="N45" s="33" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="O45" s="25" t="s">
         <v>146</v>
       </c>
       <c r="P45" s="33" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="Q45" s="25" t="s">
         <v>144</v>
@@ -6001,13 +5933,13 @@
         <v>45009</v>
       </c>
       <c r="G46" s="24" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="H46" s="35" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="I46" s="24" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="J46" s="25" t="s">
         <v>64</v>
@@ -6020,13 +5952,13 @@
         <v>64</v>
       </c>
       <c r="N46" s="33" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="O46" s="25" t="s">
         <v>146</v>
       </c>
       <c r="P46" s="33" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="Q46" s="25" t="s">
         <v>144</v>
@@ -6057,13 +5989,13 @@
         <v>45009</v>
       </c>
       <c r="G47" s="24" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="H47" s="35" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="I47" s="35" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="J47" s="25" t="s">
         <v>64</v>
@@ -6076,13 +6008,13 @@
         <v>64</v>
       </c>
       <c r="N47" s="33" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="O47" s="25" t="s">
         <v>146</v>
       </c>
       <c r="P47" s="33" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="Q47" s="25" t="s">
         <v>144</v>
@@ -6341,13 +6273,13 @@
         <v>45009</v>
       </c>
       <c r="G54" s="24" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="H54" s="24" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="I54" s="24" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="J54" s="25" t="s">
         <v>64</v>
@@ -6360,13 +6292,13 @@
         <v>64</v>
       </c>
       <c r="N54" s="25" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="O54" s="25" t="s">
         <v>146</v>
       </c>
       <c r="P54" s="25" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="Q54" s="25" t="s">
         <v>144</v>
@@ -15998,7 +15930,7 @@
           <x14:formula1>
             <xm:f>Sheet1!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>O10:O54 J16 J10:J14 J18 J20:J31 J33:J54 L10:M54</xm:sqref>
+          <xm:sqref>O10:O54 J16 J10:J14 J18 J20:J54 L10:M54</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000001000000}">
           <x14:formula1>

</xml_diff>

<commit_message>
Aggiornata check-list Come richiesto sono state dettagliate le descrizioni dei test con ID 45, 48, 63, 65, 151, 153, 169
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111BIMIND00000/BiMind/Human/10.6/report-checklist.xlsx
+++ b/GATEWAY/A1#111BIMIND00000/BiMind/Human/10.6/report-checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\ProgettiGit\it-fse-accreditamento\GATEWAY\A1#111BIMIND00000\BiMind\Human\10.6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D03C9E23-CBDA-4690-A097-4871A858A690}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BD9D28A-E0AF-4706-9869-A9BDEEC9E65C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15855" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="245">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -825,9 +825,6 @@
     <t>Errore connessione al servizio di validazione del documento. Verrà ritentata la validazione a breve. Proseguire con la firma</t>
   </si>
   <si>
-    <t xml:space="preserve"> Visualizzazione errore di connessione al servizio all'operatore. La validazione verrà ritentata in background a posteriori</t>
-  </si>
-  <si>
     <t>03093a48ffc66c8e</t>
   </si>
   <si>
@@ -835,12 +832,6 @@
   </si>
   <si>
     <t>2023-03-24T11:37:08Z</t>
-  </si>
-  <si>
-    <t>Il documento non risulta valido. Non potrà essere inviato all'FSE. Proseguire con la firma</t>
-  </si>
-  <si>
-    <t>L'errore non è gestibile a posteriori</t>
   </si>
   <si>
     <t>b03d1e8b4fbc9f30</t>
@@ -1055,6 +1046,24 @@
   </si>
   <si>
     <t>2023-04-20T12:19:20Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Visualizzazione errore di connessione al servizio all'operatore. Il documento viene inserito in una coda che si occupa di eseguire la retry in modo automatico</t>
+  </si>
+  <si>
+    <t>Il documento non risulta valido ai fini dell'invio all'FSE. Proseguire con la firma</t>
+  </si>
+  <si>
+    <t>L'errore non è gestibile a posteriori. In questo caso d'uso il documento non verrà inviato all'FSE</t>
+  </si>
+  <si>
+    <t>Si precisa che l'errore in oggetto non può verificarsi a meno di un'errore di configurazione del sistema. In tale caso la risoluzione richiederebbe un intervento tecnico</t>
+  </si>
+  <si>
+    <t>Si precisa che l'errore in oggetto non può verificarsi perché il valore "Restricted" non può essere scelto dall'utente</t>
+  </si>
+  <si>
+    <t>Si precisa che l'errore in oggetto non può verificarsi perché non è possibile valorizzare legalAuthenticator con un codice diverso da "S"</t>
   </si>
 </sst>
 </file>
@@ -1386,7 +1395,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1512,6 +1521,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1835,7 +1850,7 @@
     </row>
     <row r="4" spans="1:1" ht="14.25" customHeight="1">
       <c r="A4" s="37" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="14.25" customHeight="1">
@@ -3971,13 +3986,14 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:T672"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="Q13" sqref="Q13"/>
+      <selection pane="bottomRight" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -4231,7 +4247,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="150.75" thickBot="1">
+    <row r="10" spans="1:20" ht="150.75" hidden="1" thickBot="1">
       <c r="A10" s="20">
         <v>6</v>
       </c>
@@ -4269,7 +4285,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="150.75" thickBot="1">
+    <row r="11" spans="1:20" ht="150.75" hidden="1" thickBot="1">
       <c r="A11" s="20">
         <v>7</v>
       </c>
@@ -4307,7 +4323,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="150.75" thickBot="1">
+    <row r="12" spans="1:20" ht="150.75" hidden="1" thickBot="1">
       <c r="A12" s="20">
         <v>8</v>
       </c>
@@ -4345,7 +4361,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="150.75" thickBot="1">
+    <row r="13" spans="1:20" ht="150.75" hidden="1" thickBot="1">
       <c r="A13" s="20">
         <v>9</v>
       </c>
@@ -4383,7 +4399,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="150.75" thickBot="1">
+    <row r="14" spans="1:20" ht="150.75" hidden="1" thickBot="1">
       <c r="A14" s="20">
         <v>29</v>
       </c>
@@ -4403,10 +4419,10 @@
         <v>45036</v>
       </c>
       <c r="G14" s="24" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="H14" s="24" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="I14" s="24"/>
       <c r="J14" s="25" t="s">
@@ -4435,7 +4451,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="150.75" thickBot="1">
+    <row r="15" spans="1:20" ht="150.75" hidden="1" thickBot="1">
       <c r="A15" s="20">
         <v>32</v>
       </c>
@@ -4455,10 +4471,10 @@
         <v>45036</v>
       </c>
       <c r="G15" s="24" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="H15" s="24" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="I15" s="24"/>
       <c r="J15" s="25" t="s">
@@ -4487,7 +4503,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="165.75" thickBot="1">
+    <row r="16" spans="1:20" ht="165.75" hidden="1" thickBot="1">
       <c r="A16" s="20">
         <v>37</v>
       </c>
@@ -4507,10 +4523,10 @@
         <v>45036</v>
       </c>
       <c r="G16" s="24" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="H16" s="24" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="I16" s="24"/>
       <c r="J16" s="25" t="s">
@@ -4539,7 +4555,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="165.75" thickBot="1">
+    <row r="17" spans="1:20" ht="165.75" hidden="1" thickBot="1">
       <c r="A17" s="20">
         <v>40</v>
       </c>
@@ -4559,10 +4575,10 @@
         <v>45036</v>
       </c>
       <c r="G17" s="24" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="H17" s="24" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="I17" s="24"/>
       <c r="J17" s="25" t="s">
@@ -4591,7 +4607,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="75.75" thickBot="1">
+    <row r="18" spans="1:20" ht="90.75" hidden="1" thickBot="1">
       <c r="A18" s="20">
         <v>45</v>
       </c>
@@ -4627,8 +4643,8 @@
       <c r="O18" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="P18" s="25" t="s">
-        <v>168</v>
+      <c r="P18" s="33" t="s">
+        <v>239</v>
       </c>
       <c r="Q18" s="25" t="s">
         <v>144</v>
@@ -4641,7 +4657,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="75.75" thickBot="1">
+    <row r="19" spans="1:20" ht="90.75" hidden="1" thickBot="1">
       <c r="A19" s="20">
         <v>48</v>
       </c>
@@ -4677,8 +4693,8 @@
       <c r="O19" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="P19" s="25" t="s">
-        <v>168</v>
+      <c r="P19" s="33" t="s">
+        <v>239</v>
       </c>
       <c r="Q19" s="25" t="s">
         <v>144</v>
@@ -4704,20 +4720,20 @@
       <c r="D20" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="E20" s="22" t="s">
+      <c r="E20" s="50" t="s">
         <v>68</v>
       </c>
       <c r="F20" s="23">
         <v>45010</v>
       </c>
       <c r="G20" s="24" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="H20" s="24" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="I20" s="24" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J20" s="25" t="s">
         <v>64</v>
@@ -4729,25 +4745,27 @@
       <c r="M20" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="N20" s="25" t="s">
-        <v>172</v>
+      <c r="N20" s="33" t="s">
+        <v>240</v>
       </c>
       <c r="O20" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="P20" s="25" t="s">
-        <v>173</v>
+      <c r="P20" s="33" t="s">
+        <v>241</v>
       </c>
       <c r="Q20" s="25" t="s">
         <v>144</v>
       </c>
       <c r="R20" s="26"/>
-      <c r="S20" s="27"/>
+      <c r="S20" s="51" t="s">
+        <v>242</v>
+      </c>
       <c r="T20" s="28" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="120.75" thickBot="1">
+    <row r="21" spans="1:20" ht="120.75" hidden="1" thickBot="1">
       <c r="A21" s="20">
         <v>64</v>
       </c>
@@ -4767,13 +4785,13 @@
         <v>45010</v>
       </c>
       <c r="G21" s="24" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="H21" s="24" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="I21" s="24" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="J21" s="25" t="s">
         <v>64</v>
@@ -4786,13 +4804,13 @@
         <v>64</v>
       </c>
       <c r="N21" s="25" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="O21" s="25" t="s">
         <v>146</v>
       </c>
       <c r="P21" s="25" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="Q21" s="25" t="s">
         <v>144</v>
@@ -4823,13 +4841,13 @@
         <v>45010</v>
       </c>
       <c r="G22" s="24" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="H22" s="24" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="I22" s="24" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="J22" s="25" t="s">
         <v>64</v>
@@ -4842,24 +4860,26 @@
         <v>64</v>
       </c>
       <c r="N22" s="25" t="s">
-        <v>172</v>
+        <v>240</v>
       </c>
       <c r="O22" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="P22" s="25" t="s">
-        <v>173</v>
+      <c r="P22" s="33" t="s">
+        <v>241</v>
       </c>
       <c r="Q22" s="25" t="s">
         <v>144</v>
       </c>
       <c r="R22" s="26"/>
-      <c r="S22" s="27"/>
+      <c r="S22" s="51" t="s">
+        <v>243</v>
+      </c>
       <c r="T22" s="28" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="120.75" thickBot="1">
+    <row r="23" spans="1:20" ht="120.75" hidden="1" thickBot="1">
       <c r="A23" s="20">
         <v>66</v>
       </c>
@@ -4897,7 +4917,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="120.75" thickBot="1">
+    <row r="24" spans="1:20" ht="120.75" hidden="1" thickBot="1">
       <c r="A24" s="20">
         <v>67</v>
       </c>
@@ -4917,13 +4937,13 @@
         <v>45010</v>
       </c>
       <c r="G24" s="24" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="H24" s="24" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="I24" s="24" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="J24" s="25" t="s">
         <v>64</v>
@@ -4936,13 +4956,13 @@
         <v>64</v>
       </c>
       <c r="N24" s="25" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="O24" s="25" t="s">
         <v>146</v>
       </c>
       <c r="P24" s="25" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="Q24" s="25" t="s">
         <v>144</v>
@@ -4953,7 +4973,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="120.75" thickBot="1">
+    <row r="25" spans="1:20" ht="120.75" hidden="1" thickBot="1">
       <c r="A25" s="20">
         <v>68</v>
       </c>
@@ -4973,13 +4993,13 @@
         <v>45010</v>
       </c>
       <c r="G25" s="24" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="H25" s="24" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="I25" s="24" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="J25" s="25" t="s">
         <v>64</v>
@@ -4992,13 +5012,13 @@
         <v>64</v>
       </c>
       <c r="N25" s="33" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="O25" s="25" t="s">
         <v>146</v>
       </c>
       <c r="P25" s="25" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="Q25" s="25" t="s">
         <v>144</v>
@@ -5009,7 +5029,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="120.75" thickBot="1">
+    <row r="26" spans="1:20" ht="120.75" hidden="1" thickBot="1">
       <c r="A26" s="20">
         <v>69</v>
       </c>
@@ -5029,13 +5049,13 @@
         <v>45010</v>
       </c>
       <c r="G26" s="24" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="H26" s="24" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="I26" s="24" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="J26" s="25" t="s">
         <v>64</v>
@@ -5048,13 +5068,13 @@
         <v>64</v>
       </c>
       <c r="N26" s="33" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="O26" s="25" t="s">
         <v>146</v>
       </c>
       <c r="P26" s="33" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="Q26" s="25" t="s">
         <v>144</v>
@@ -5065,7 +5085,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="120.75" thickBot="1">
+    <row r="27" spans="1:20" ht="120.75" hidden="1" thickBot="1">
       <c r="A27" s="20">
         <v>70</v>
       </c>
@@ -5085,13 +5105,13 @@
         <v>45010</v>
       </c>
       <c r="G27" s="24" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="H27" s="24" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="I27" s="24" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="J27" s="25" t="s">
         <v>64</v>
@@ -5104,13 +5124,13 @@
         <v>64</v>
       </c>
       <c r="N27" s="33" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="O27" s="25" t="s">
         <v>146</v>
       </c>
       <c r="P27" s="33" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="Q27" s="25" t="s">
         <v>144</v>
@@ -5121,7 +5141,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="120.75" thickBot="1">
+    <row r="28" spans="1:20" ht="120.75" hidden="1" thickBot="1">
       <c r="A28" s="20">
         <v>71</v>
       </c>
@@ -5159,7 +5179,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="120.75" thickBot="1">
+    <row r="29" spans="1:20" ht="120.75" hidden="1" thickBot="1">
       <c r="A29" s="20">
         <v>72</v>
       </c>
@@ -5197,7 +5217,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="120.75" thickBot="1">
+    <row r="30" spans="1:20" ht="120.75" hidden="1" thickBot="1">
       <c r="A30" s="20">
         <v>73</v>
       </c>
@@ -5235,7 +5255,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="120.75" thickBot="1">
+    <row r="31" spans="1:20" ht="120.75" hidden="1" thickBot="1">
       <c r="A31" s="20">
         <v>74</v>
       </c>
@@ -5273,7 +5293,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="165.75" thickBot="1">
+    <row r="32" spans="1:20" ht="165.75" hidden="1" thickBot="1">
       <c r="A32" s="20">
         <v>147</v>
       </c>
@@ -5311,7 +5331,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="33" spans="1:20" ht="165.75" thickBot="1">
+    <row r="33" spans="1:20" ht="165.75" hidden="1" thickBot="1">
       <c r="A33" s="20">
         <v>148</v>
       </c>
@@ -5349,7 +5369,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="165.75" thickBot="1">
+    <row r="34" spans="1:20" ht="165.75" hidden="1" thickBot="1">
       <c r="A34" s="20">
         <v>149</v>
       </c>
@@ -5387,7 +5407,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="35" spans="1:20" ht="165.75" thickBot="1">
+    <row r="35" spans="1:20" ht="165.75" hidden="1" thickBot="1">
       <c r="A35" s="20">
         <v>150</v>
       </c>
@@ -5445,13 +5465,13 @@
         <v>45009</v>
       </c>
       <c r="G36" s="24" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H36" s="24" t="s">
+        <v>168</v>
+      </c>
+      <c r="I36" s="24" t="s">
         <v>169</v>
-      </c>
-      <c r="I36" s="24" t="s">
-        <v>170</v>
       </c>
       <c r="J36" s="25" t="s">
         <v>64</v>
@@ -5464,24 +5484,26 @@
         <v>64</v>
       </c>
       <c r="N36" s="25" t="s">
-        <v>172</v>
+        <v>240</v>
       </c>
       <c r="O36" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="P36" s="25" t="s">
-        <v>173</v>
+      <c r="P36" s="33" t="s">
+        <v>241</v>
       </c>
       <c r="Q36" s="25" t="s">
         <v>144</v>
       </c>
       <c r="R36" s="26"/>
-      <c r="S36" s="27"/>
+      <c r="S36" s="51" t="s">
+        <v>242</v>
+      </c>
       <c r="T36" s="28" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="37" spans="1:20" ht="135.75" thickBot="1">
+    <row r="37" spans="1:20" ht="135.75" hidden="1" thickBot="1">
       <c r="A37" s="20">
         <v>152</v>
       </c>
@@ -5501,13 +5523,13 @@
         <v>45009</v>
       </c>
       <c r="G37" s="24" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="H37" s="24" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="I37" s="24" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="J37" s="25" t="s">
         <v>64</v>
@@ -5520,13 +5542,13 @@
         <v>64</v>
       </c>
       <c r="N37" s="25" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="O37" s="25" t="s">
         <v>146</v>
       </c>
       <c r="P37" s="25" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="Q37" s="25" t="s">
         <v>144</v>
@@ -5557,13 +5579,13 @@
         <v>45009</v>
       </c>
       <c r="G38" s="24" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="H38" s="24" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="I38" s="24" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="J38" s="25" t="s">
         <v>64</v>
@@ -5576,24 +5598,26 @@
         <v>64</v>
       </c>
       <c r="N38" s="25" t="s">
-        <v>172</v>
+        <v>240</v>
       </c>
       <c r="O38" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="P38" s="25" t="s">
-        <v>173</v>
+      <c r="P38" s="33" t="s">
+        <v>241</v>
       </c>
       <c r="Q38" s="25" t="s">
         <v>144</v>
       </c>
       <c r="R38" s="26"/>
-      <c r="S38" s="27"/>
+      <c r="S38" s="51" t="s">
+        <v>243</v>
+      </c>
       <c r="T38" s="28" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="39" spans="1:20" ht="135.75" thickBot="1">
+    <row r="39" spans="1:20" ht="135" hidden="1">
       <c r="A39" s="20">
         <v>154</v>
       </c>
@@ -5631,7 +5655,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="40" spans="1:20" ht="135.75" thickBot="1">
+    <row r="40" spans="1:20" ht="135" hidden="1">
       <c r="A40" s="20">
         <v>155</v>
       </c>
@@ -5651,13 +5675,13 @@
         <v>45009</v>
       </c>
       <c r="G40" s="24" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="H40" s="24" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="I40" s="24" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="J40" s="25" t="s">
         <v>64</v>
@@ -5670,13 +5694,13 @@
         <v>64</v>
       </c>
       <c r="N40" s="25" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="O40" s="25" t="s">
         <v>146</v>
       </c>
       <c r="P40" s="25" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="Q40" s="25" t="s">
         <v>144</v>
@@ -5687,7 +5711,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="41" spans="1:20" ht="135.75" thickBot="1">
+    <row r="41" spans="1:20" ht="135" hidden="1">
       <c r="A41" s="20">
         <v>156</v>
       </c>
@@ -5707,13 +5731,13 @@
         <v>45009</v>
       </c>
       <c r="G41" s="24" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="H41" s="24" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="I41" s="24" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="J41" s="25" t="s">
         <v>64</v>
@@ -5726,13 +5750,13 @@
         <v>64</v>
       </c>
       <c r="N41" s="33" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="O41" s="25" t="s">
         <v>146</v>
       </c>
       <c r="P41" s="25" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="Q41" s="25" t="s">
         <v>144</v>
@@ -5743,7 +5767,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="42" spans="1:20" ht="135.75" thickBot="1">
+    <row r="42" spans="1:20" ht="135" hidden="1">
       <c r="A42" s="20">
         <v>157</v>
       </c>
@@ -5781,7 +5805,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="43" spans="1:20" ht="135.75" thickBot="1">
+    <row r="43" spans="1:20" ht="135" hidden="1">
       <c r="A43" s="20">
         <v>158</v>
       </c>
@@ -5819,7 +5843,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="44" spans="1:20" ht="120.75" thickBot="1">
+    <row r="44" spans="1:20" ht="120" hidden="1">
       <c r="A44" s="20">
         <v>159</v>
       </c>
@@ -5857,7 +5881,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="45" spans="1:20" ht="120.75" thickBot="1">
+    <row r="45" spans="1:20" ht="120" hidden="1">
       <c r="A45" s="20">
         <v>160</v>
       </c>
@@ -5877,13 +5901,13 @@
         <v>45009</v>
       </c>
       <c r="G45" s="24" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="H45" s="24" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="I45" s="24" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="J45" s="25" t="s">
         <v>64</v>
@@ -5896,13 +5920,13 @@
         <v>64</v>
       </c>
       <c r="N45" s="33" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="O45" s="25" t="s">
         <v>146</v>
       </c>
       <c r="P45" s="33" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="Q45" s="25" t="s">
         <v>144</v>
@@ -5913,7 +5937,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:20" ht="135.75" thickBot="1">
+    <row r="46" spans="1:20" ht="135" hidden="1">
       <c r="A46" s="20">
         <v>161</v>
       </c>
@@ -5933,13 +5957,13 @@
         <v>45009</v>
       </c>
       <c r="G46" s="24" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="H46" s="35" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="I46" s="24" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="J46" s="25" t="s">
         <v>64</v>
@@ -5952,13 +5976,13 @@
         <v>64</v>
       </c>
       <c r="N46" s="33" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="O46" s="25" t="s">
         <v>146</v>
       </c>
       <c r="P46" s="33" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="Q46" s="25" t="s">
         <v>144</v>
@@ -5969,7 +5993,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:20" ht="135.75" thickBot="1">
+    <row r="47" spans="1:20" ht="135" hidden="1">
       <c r="A47" s="20">
         <v>162</v>
       </c>
@@ -5989,13 +6013,13 @@
         <v>45009</v>
       </c>
       <c r="G47" s="24" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="H47" s="35" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="I47" s="35" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="J47" s="25" t="s">
         <v>64</v>
@@ -6008,13 +6032,13 @@
         <v>64</v>
       </c>
       <c r="N47" s="33" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="O47" s="25" t="s">
         <v>146</v>
       </c>
       <c r="P47" s="33" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="Q47" s="25" t="s">
         <v>144</v>
@@ -6025,7 +6049,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="48" spans="1:20" ht="135.75" thickBot="1">
+    <row r="48" spans="1:20" ht="135" hidden="1">
       <c r="A48" s="20">
         <v>163</v>
       </c>
@@ -6063,7 +6087,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="49" spans="1:20" ht="135.75" thickBot="1">
+    <row r="49" spans="1:20" ht="135" hidden="1">
       <c r="A49" s="20">
         <v>164</v>
       </c>
@@ -6101,7 +6125,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="50" spans="1:20" ht="135.75" thickBot="1">
+    <row r="50" spans="1:20" ht="135" hidden="1">
       <c r="A50" s="20">
         <v>165</v>
       </c>
@@ -6139,7 +6163,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="51" spans="1:20" ht="135.75" thickBot="1">
+    <row r="51" spans="1:20" ht="135" hidden="1">
       <c r="A51" s="20">
         <v>166</v>
       </c>
@@ -6177,7 +6201,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="52" spans="1:20" ht="135.75" thickBot="1">
+    <row r="52" spans="1:20" ht="135" hidden="1">
       <c r="A52" s="20">
         <v>167</v>
       </c>
@@ -6215,7 +6239,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="53" spans="1:20" ht="135.75" thickBot="1">
+    <row r="53" spans="1:20" ht="135" hidden="1">
       <c r="A53" s="20">
         <v>168</v>
       </c>
@@ -6273,13 +6297,13 @@
         <v>45009</v>
       </c>
       <c r="G54" s="24" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="H54" s="24" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="I54" s="24" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="J54" s="25" t="s">
         <v>64</v>
@@ -6292,19 +6316,21 @@
         <v>64</v>
       </c>
       <c r="N54" s="25" t="s">
-        <v>172</v>
+        <v>240</v>
       </c>
       <c r="O54" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="P54" s="25" t="s">
-        <v>173</v>
+      <c r="P54" s="33" t="s">
+        <v>241</v>
       </c>
       <c r="Q54" s="25" t="s">
         <v>144</v>
       </c>
       <c r="R54" s="26"/>
-      <c r="S54" s="27"/>
+      <c r="S54" s="51" t="s">
+        <v>244</v>
+      </c>
       <c r="T54" s="28" t="s">
         <v>44</v>
       </c>
@@ -15907,6 +15933,15 @@
     </row>
   </sheetData>
   <autoFilter ref="A9:T54" xr:uid="{00000000-0009-0000-0000-000002000000}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="151"/>
+        <filter val="153"/>
+        <filter val="169"/>
+        <filter val="63"/>
+        <filter val="65"/>
+      </filters>
+    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A9:T54">
       <sortCondition ref="B9:B54"/>
     </sortState>

</xml_diff>